<commit_message>
Atualização de Todos os Documentos da Sprint 3
</commit_message>
<xml_diff>
--- a/Sprint-3/Product Backlog-Burndown.xlsx
+++ b/Sprint-3/Product Backlog-Burndown.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\breno\Downloads\adocao4\Sprint-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Adocao\adocao\Sprint-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Product Burndown" sheetId="2" r:id="rId2"/>
     <sheet name="Lista de tarefas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -199,9 +199,6 @@
     <t>Criação do diagrama de classe.</t>
   </si>
   <si>
-    <t>Usuário que desejam adotar um animal, devem preencher um formulário de cadastro no sistema, e posteriormente enviar para um administrador</t>
-  </si>
-  <si>
     <t>Um candidado precisa realizar o cadastro com todas suas informações para solicitar a adoção do animal</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>Estudo Engenharia de Requisitos</t>
   </si>
   <si>
-    <t>Usuário que desejam adotar um animal, poderão ver uma lista de animais disponível para adoção</t>
-  </si>
-  <si>
     <t>Ao visualizar todos os animais disponíveis para a adoção, bem como suas informações, o usuário poderá clicar no botão "Adotar" para que possa se iniciar o processo de adoção</t>
   </si>
   <si>
@@ -266,16 +260,22 @@
   </si>
   <si>
     <t>Criar visualização da Lista de Animais</t>
+  </si>
+  <si>
+    <t>O Usuário que deseja adotar um animal, deve preencher um formulário de cadastro no sistema, e posteriormente enviar para um administrador</t>
+  </si>
+  <si>
+    <t>Para que um  usuário adote um animal, é necessário visualizar uma lista dos animais que estão disponíveis para adoção</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -361,13 +361,6 @@
       <family val="1"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="0"/>
@@ -375,14 +368,8 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +422,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF003366"/>
       </patternFill>
     </fill>
   </fills>
@@ -546,7 +539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -617,13 +610,10 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -638,9 +628,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -662,13 +649,7 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -689,10 +670,16 @@
     <xf numFmtId="164" fontId="8" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -827,7 +814,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -874,7 +861,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -923,12 +910,15 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6672-459F-9697-9E0FFD9903C1}"/>
+            </c:ext>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>label 0</c15:sqref>
@@ -949,7 +939,7 @@
               <c15:filteredCategoryTitle>
                 <c15:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>categories</c15:sqref>
@@ -996,9 +986,6 @@
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6672-459F-9697-9E0FFD9903C1}"/>
-            </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
@@ -1036,7 +1023,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1085,12 +1072,15 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6672-459F-9697-9E0FFD9903C1}"/>
+            </c:ext>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:filteredSeriesTitle>
                 <c15:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>label 1</c15:sqref>
@@ -1111,7 +1101,7 @@
               <c15:filteredCategoryTitle>
                 <c15:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>categories</c15:sqref>
@@ -1158,9 +1148,6 @@
                 </c15:cat>
               </c15:filteredCategoryTitle>
             </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-6672-459F-9697-9E0FFD9903C1}"/>
-            </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
@@ -1180,11 +1167,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1550343200"/>
-        <c:axId val="1550340480"/>
+        <c:axId val="1809067872"/>
+        <c:axId val="1809077120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1550343200"/>
+        <c:axId val="1809067872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1219,7 +1206,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1550340480"/>
+        <c:crossAx val="1809077120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1227,7 +1214,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1550340480"/>
+        <c:axId val="1809077120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
@@ -1273,7 +1260,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1550343200"/>
+        <c:crossAx val="1809067872"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1286,7 +1273,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1351,7 +1337,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1389,7 +1375,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1461,7 +1447,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1613,8 +1599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1048570"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C27" sqref="C25:C27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1629,14 +1615,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -1741,10 +1727,10 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="36" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="24" t="s">
@@ -1774,8 +1760,8 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="39"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="48"/>
       <c r="C6" s="24" t="s">
         <v>55</v>
       </c>
@@ -1803,8 +1789,8 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
-      <c r="B7" s="43"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="25" t="s">
         <v>56</v>
       </c>
@@ -1832,10 +1818,10 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="32" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1865,8 +1851,8 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="32"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="4" t="s">
         <v>44</v>
       </c>
@@ -1894,8 +1880,8 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
-      <c r="B10" s="35"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="5" t="s">
         <v>45</v>
       </c>
@@ -1923,12 +1909,12 @@
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="6">
         <v>3</v>
       </c>
       <c r="E11" s="6">
@@ -1952,8 +1938,8 @@
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="7" t="s">
         <v>47</v>
       </c>
@@ -1981,8 +1967,8 @@
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="7" t="s">
         <v>48</v>
       </c>
@@ -2010,8 +1996,8 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="7" t="s">
         <v>43</v>
       </c>
@@ -2039,8 +2025,8 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
@@ -2068,14 +2054,14 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="C16" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="D16" s="6">
         <v>1</v>
@@ -2101,10 +2087,10 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="32"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
@@ -2130,10 +2116,10 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="32"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="6">
         <v>0.5</v>
@@ -2159,12 +2145,12 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="32"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="47"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="26">
+        <v>61</v>
+      </c>
+      <c r="D19" s="6">
         <v>2</v>
       </c>
       <c r="E19" s="6">
@@ -2188,10 +2174,10 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="32"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="33"/>
       <c r="C20" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="6">
         <v>0.3</v>
@@ -2217,10 +2203,10 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="32"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" s="6">
         <v>1</v>
@@ -2246,10 +2232,10 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="32"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="6">
         <v>4</v>
@@ -2275,10 +2261,10 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="32"/>
-      <c r="B23" s="35"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="6">
         <v>1</v>
@@ -2304,10 +2290,10 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="33"/>
-      <c r="B24" s="36"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="6">
         <v>1</v>
@@ -2332,15 +2318,15 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="31" t="s">
+    <row r="25" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>75</v>
-      </c>
-      <c r="B25" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>77</v>
       </c>
       <c r="D25" s="6">
         <v>1</v>
@@ -2365,11 +2351,11 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="32"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="29" t="s">
-        <v>78</v>
+    <row r="26" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="31"/>
+      <c r="B26" s="33"/>
+      <c r="C26" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="D26" s="6">
         <v>1.5</v>
@@ -2394,11 +2380,11 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="32"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="29" t="s">
-        <v>79</v>
+    <row r="27" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="31"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="28" t="s">
+        <v>77</v>
       </c>
       <c r="D27" s="6">
         <v>2</v>
@@ -2424,14 +2410,14 @@
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="34" t="s">
+      <c r="C28" s="28" t="s">
         <v>69</v>
-      </c>
-      <c r="C28" s="29" t="s">
-        <v>70</v>
       </c>
       <c r="D28" s="6">
         <v>2</v>
@@ -2457,10 +2443,10 @@
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="35"/>
-      <c r="B29" s="35"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D29" s="6">
         <v>2</v>
@@ -2486,10 +2472,10 @@
       <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="35"/>
-      <c r="B30" s="35"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30" s="6">
         <v>2</v>
@@ -2515,10 +2501,10 @@
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="35"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="30" t="s">
-        <v>74</v>
+      <c r="A31" s="33"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="29" t="s">
+        <v>73</v>
       </c>
       <c r="D31" s="6">
         <v>2</v>
@@ -2544,10 +2530,10 @@
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="30" t="s">
-        <v>73</v>
+      <c r="A32" s="34"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="29" t="s">
+        <v>72</v>
       </c>
       <c r="D32" s="6">
         <v>2</v>
@@ -2573,7 +2559,7 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="3"/>
@@ -2596,7 +2582,7 @@
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="28"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
@@ -2728,20 +2714,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46" t="s">
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
       <c r="M1" s="12"/>
       <c r="N1" s="12"/>
       <c r="O1" s="1"/>
@@ -2756,40 +2742,40 @@
       <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="J2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="50" t="s">
+      <c r="L2" s="39" t="s">
         <v>22</v>
       </c>
       <c r="O2" s="1"/>
@@ -2804,18 +2790,18 @@
       <c r="X2" s="1"/>
     </row>
     <row r="3" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
@@ -3003,22 +2989,22 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
       <c r="M8" s="20" t="s">
         <v>9</v>
       </c>
@@ -3037,10 +3023,10 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="45">
+      <c r="A9" s="41">
         <v>50</v>
       </c>
-      <c r="B9" s="45"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="18">
         <f>SUMIF('Product Backlog'!F:F,1,'Product Backlog'!E:E)</f>
         <v>35</v>
@@ -3102,6 +3088,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="C8:L8"/>
@@ -3118,7 +3105,6 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <conditionalFormatting sqref="C10:N91">
     <cfRule type="expression" dxfId="2" priority="2">

</xml_diff>